<commit_message>
modified:   Sports_I_Did.xlsx 	modified:   index.html
</commit_message>
<xml_diff>
--- a/Sports_I_Did.xlsx
+++ b/Sports_I_Did.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uctcloud-my.sharepoint.com/personal/smsmoe006_myuct_ac_za/Documents/Third Year(2025)/Projects/Website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="8_{1964EA4D-03C3-4E12-B54B-E761AA3B029F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FD3262C3-FFB4-4DD3-9DEA-394CDBDD2582}"/>
+  <xr:revisionPtr revIDLastSave="118" documentId="8_{1964EA4D-03C3-4E12-B54B-E761AA3B029F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DEEAB36E-BA84-4268-A874-950DB3765F78}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A05F58E4-3C7C-4BE2-B2F5-FFDED2EF2988}"/>
+    <workbookView xWindow="2124" yWindow="1812" windowWidth="11472" windowHeight="9564" xr2:uid="{A05F58E4-3C7C-4BE2-B2F5-FFDED2EF2988}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="54">
   <si>
     <t>Archery</t>
   </si>
@@ -83,9 +83,6 @@
     <t>Chess</t>
   </si>
   <si>
-    <t>Checkers</t>
-  </si>
-  <si>
     <t>Badminton</t>
   </si>
   <si>
@@ -104,10 +101,103 @@
     <t>Description</t>
   </si>
   <si>
-    <t>None</t>
-  </si>
-  <si>
-    <t>I use the heaviest bow in the club</t>
+    <t>Started</t>
+  </si>
+  <si>
+    <t>I use the 35lb left-hand bow</t>
+  </si>
+  <si>
+    <t>Captain of the team</t>
+  </si>
+  <si>
+    <t>Started for Assassins</t>
+  </si>
+  <si>
+    <t>I started to learn the sport and was quite a noob</t>
+  </si>
+  <si>
+    <t>After many months of hard work, I was recognized for it and became a leader</t>
+  </si>
+  <si>
+    <t>Coach and Captain</t>
+  </si>
+  <si>
+    <t>Was the coach and captain of College House Residence for the interleague</t>
+  </si>
+  <si>
+    <t>2023 - 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Runner-Up </t>
+  </si>
+  <si>
+    <t>Came 2nd Place for 3 v 3 Tournament</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Came 2nd Place for my division </t>
+  </si>
+  <si>
+    <t>Hobby</t>
+  </si>
+  <si>
+    <t>Tried the sport out to learn about it.</t>
+  </si>
+  <si>
+    <t>Ongoing</t>
+  </si>
+  <si>
+    <t>Continue to grow my skills</t>
+  </si>
+  <si>
+    <t>Tried the sport out to learn about it. And nickname the Piosoner for my serves.</t>
+  </si>
+  <si>
+    <t>2015 - 2019</t>
+  </si>
+  <si>
+    <t>Tried the sport but I am no good.</t>
+  </si>
+  <si>
+    <t>Not the best at it and not my favourite</t>
+  </si>
+  <si>
+    <t>For Fun</t>
+  </si>
+  <si>
+    <t>I played against my high school netball team and classmates, and I was a very good shooter (thanks to basketball). My basketball mates and I had to play for the court and winner gets the court.</t>
+  </si>
+  <si>
+    <t>Self-Defense and Discipline</t>
+  </si>
+  <si>
+    <t>Discipline. To help meditate.</t>
+  </si>
+  <si>
+    <t>Father use to teach me how to box with punching bag.</t>
+  </si>
+  <si>
+    <t>Was very good with receiver. And went to a boot camp just to get some workout in.</t>
+  </si>
+  <si>
+    <t>2019 - 2020</t>
+  </si>
+  <si>
+    <t>I played at College House Pool table for fun.</t>
+  </si>
+  <si>
+    <t>I was taught by my father and joined a school chess team.</t>
+  </si>
+  <si>
+    <t>I won every game on my team and became a leader. But overall my team came second.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">University </t>
+  </si>
+  <si>
+    <t>Join College House team</t>
+  </si>
+  <si>
+    <t>Average ELO Rating of 1500</t>
   </si>
 </sst>
 </file>
@@ -479,32 +569,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21923149-7A90-4DC2-950F-DE54F4C53C84}">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="16.109375" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" customWidth="1"/>
     <col min="3" max="3" width="16.6640625" customWidth="1"/>
-    <col min="4" max="4" width="18.44140625" customWidth="1"/>
+    <col min="4" max="4" width="74.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
         <v>18</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>19</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>20</v>
-      </c>
-      <c r="D1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -512,98 +602,321 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C2">
         <v>2025</v>
       </c>
       <c r="D2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3">
+        <v>2018</v>
+      </c>
+      <c r="D3" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4">
+        <v>2020</v>
+      </c>
+      <c r="D4" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5">
+        <v>2020</v>
+      </c>
+      <c r="D5" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7">
+        <v>2019</v>
+      </c>
+      <c r="D7" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>2</v>
+      </c>
+      <c r="B8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>4</v>
+      </c>
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9">
+        <v>2024</v>
+      </c>
+      <c r="D9" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>5</v>
+      </c>
+      <c r="B10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10">
+        <v>2019</v>
+      </c>
+      <c r="D10" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>6</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11">
+        <v>2017</v>
+      </c>
+      <c r="D11" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>7</v>
+      </c>
+      <c r="B12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>8</v>
+      </c>
+      <c r="B13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13">
+        <v>2018</v>
+      </c>
+      <c r="D13" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>9</v>
+      </c>
+      <c r="B14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14">
+        <v>2019</v>
+      </c>
+      <c r="D14" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>10</v>
+      </c>
+      <c r="B15" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15">
+        <v>2024</v>
+      </c>
+      <c r="D15" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+      <c r="B16" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16">
+        <v>2024</v>
+      </c>
+      <c r="D16" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+      <c r="B17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17">
+        <v>2017</v>
+      </c>
+      <c r="D17" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+      <c r="B18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" t="s">
+        <v>47</v>
+      </c>
+      <c r="D18" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>15</v>
+      </c>
+      <c r="B19" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19">
+        <v>2024</v>
+      </c>
+      <c r="D19" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20">
+        <v>2024</v>
+      </c>
+      <c r="D20" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>14</v>
+      </c>
+      <c r="B21" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21">
+        <v>2016</v>
+      </c>
+      <c r="D21" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>14</v>
+      </c>
+      <c r="B22" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22">
+        <v>2016</v>
+      </c>
+      <c r="D22" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>14</v>
+      </c>
+      <c r="B23" t="s">
+        <v>51</v>
+      </c>
+      <c r="C23" t="s">
+        <v>29</v>
+      </c>
+      <c r="D23" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>14</v>
+      </c>
+      <c r="B24" t="s">
+        <v>33</v>
+      </c>
+      <c r="C24" t="s">
+        <v>35</v>
+      </c>
+      <c r="D24" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>